<commit_message>
Add alert on xlsx anomly on update and add event
</commit_message>
<xml_diff>
--- a/public/files/groceries.xlsx
+++ b/public/files/groceries.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjtouuMqwG0bK5/oJbAJ9zLkZm8GQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjeNIvwUBlcniPC+tiz+dbv75UrjQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -24,7 +24,7 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Eg</t>
+    <t>Whole Eg</t>
   </si>
   <si>
     <t>Shelf stable fish and seafood</t>
@@ -53,44 +53,20 @@
     <t>Canned vegetables</t>
   </si>
   <si>
-    <t>Pet food</t>
-  </si>
-  <si>
-    <t>Roasted coffee</t>
-  </si>
-  <si>
     <t>Potatoes</t>
   </si>
   <si>
     <t>Bakery products</t>
-  </si>
-  <si>
-    <t>Propane, kerosene and firewood</t>
-  </si>
-  <si>
-    <t>Flour and prepared flour mixes</t>
-  </si>
-  <si>
-    <t>Bacon and related products</t>
-  </si>
-  <si>
-    <t>Fresh, whole chicken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
-      <sz val="14.0"/>
-      <color rgb="FF555555"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -100,7 +76,12 @@
     <font>
       <sz val="14.0"/>
       <color rgb="FF555555"/>
-      <name val="PublicoText"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14.0"/>
+      <color rgb="FF555555"/>
+      <name val="Publicotext"/>
     </font>
   </fonts>
   <fills count="3">
@@ -123,25 +104,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -360,23 +332,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="36.14"/>
     <col customWidth="1" min="2" max="2" width="32.29"/>
-    <col customWidth="1" min="3" max="3" width="16.71"/>
-    <col customWidth="1" min="4" max="4" width="12.29"/>
-    <col customWidth="1" min="5" max="5" width="13.43"/>
-    <col customWidth="1" min="6" max="6" width="19.0"/>
-    <col customWidth="1" min="7" max="7" width="10.43"/>
-    <col customWidth="1" min="8" max="8" width="18.0"/>
-    <col customWidth="1" min="9" max="9" width="13.43"/>
-    <col customWidth="1" min="10" max="10" width="7.14"/>
-    <col customWidth="1" min="11" max="11" width="8.57"/>
-    <col customWidth="1" min="12" max="12" width="17.71"/>
-    <col customWidth="1" min="13" max="13" width="10.29"/>
-    <col customWidth="1" min="14" max="14" width="5.71"/>
-    <col customWidth="1" min="15" max="15" width="7.29"/>
-    <col customWidth="1" min="16" max="16" width="10.14"/>
-    <col customWidth="1" min="17" max="17" width="11.57"/>
-    <col customWidth="1" min="18" max="21" width="16.43"/>
-    <col customWidth="1" min="22" max="26" width="10.0"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -391,136 +346,88 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>5.0</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>5.0</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>5.0</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>5.0</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>5.0</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>12.0</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>14.0</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>14.0</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <v>12.0</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3">
-        <v>12.0</v>
+      <c r="B11" s="1">
+        <v>2.0</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="B12" s="1">
         <v>53.0</v>
-      </c>
-    </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="3">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="3">
-        <v>32.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>